<commit_message>
Minor edits and figure changes
</commit_message>
<xml_diff>
--- a/ManuscriptTables.xlsx
+++ b/ManuscriptTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellenweise/Desktop/Cloned_repositories/NbdLamprey2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ClonedRepositories\NbdLamprey2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577753AC-12D0-9148-B6A3-A98531D03929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E2B411-49A2-4E1A-8EF8-C858E41C23ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17940" windowHeight="16420" activeTab="1" xr2:uid="{3BEC1152-7282-174A-AD94-25902A3A271A}"/>
+    <workbookView xWindow="-28920" yWindow="1155" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3BEC1152-7282-174A-AD94-25902A3A271A}"/>
   </bookViews>
   <sheets>
     <sheet name="AIC_values" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="211">
   <si>
     <t>Model Name</t>
   </si>
@@ -505,9 +505,6 @@
   </si>
   <si>
     <t>biotic</t>
-  </si>
-  <si>
-    <t>environmental</t>
   </si>
   <si>
     <t>Nc and TrapToMouth models</t>
@@ -693,7 +690,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -761,6 +758,19 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -809,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -901,12 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -915,6 +919,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,44 +1254,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDA6A72-C8CA-5447-95DC-B9FA8C7754B8}">
-  <dimension ref="A1:N106"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="14.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="12.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46" t="s">
+    <row r="1" spans="1:18" s="7" customFormat="1">
+      <c r="A1" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1308,12 +1324,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="10">
         <v>37.40645</v>
@@ -1346,8 +1362,14 @@
         <f t="shared" si="0"/>
         <v>19.502690000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1370,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:H11" si="1">C4-C$14</f>
+        <f>C4-C$14</f>
         <v>0.90359000000000123</v>
       </c>
       <c r="I4" s="7">
@@ -1385,8 +1407,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1409,7 +1437,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H4:H11" si="1">C5-C$14</f>
         <v>3.8315200000000047</v>
       </c>
       <c r="I5" s="7">
@@ -1424,8 +1452,14 @@
         <f t="shared" si="0"/>
         <v>5.158999999999736E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1463,8 +1497,14 @@
         <f t="shared" si="0"/>
         <v>0.2179000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="52"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1502,8 +1542,14 @@
         <f t="shared" si="0"/>
         <v>0.18951999999999458</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1541,8 +1587,14 @@
         <f t="shared" si="0"/>
         <v>0.22419000000000011</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1570,8 +1622,14 @@
         <f t="shared" si="0"/>
         <v>2.9139999999998167E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1609,8 +1667,14 @@
         <f t="shared" si="0"/>
         <v>3.2395499999999942</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1645,13 +1709,19 @@
         <v>5.4476299999999966</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="0"/>
+        <f>F11-F$14</f>
         <v>3.097379999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
@@ -1665,7 +1735,7 @@
         <v>55.546230000000001</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="7"/>
@@ -1678,13 +1748,23 @@
         <v>2.7272299999999987</v>
       </c>
       <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1705,25 +1785,49 @@
         <v>52.819000000000003</v>
       </c>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="52"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="52"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1755,8 +1859,14 @@
       <c r="K18" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="8" t="s">
         <v>5</v>
       </c>
@@ -1794,8 +1904,14 @@
         <f t="shared" si="2"/>
         <v>0.2178000000000111</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="8" t="s">
         <v>6</v>
       </c>
@@ -1833,8 +1949,14 @@
         <f t="shared" si="2"/>
         <v>13.414900000000017</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="52"/>
+      <c r="R20" s="52"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
@@ -1872,10 +1994,16 @@
         <f t="shared" si="2"/>
         <v>12.701999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="52"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B22" s="8">
         <v>1</v>
@@ -1893,7 +2021,7 @@
         <v>160.1679</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" si="3"/>
@@ -1911,8 +2039,14 @@
         <f t="shared" si="2"/>
         <v>13.126200000000011</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="52"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="8" t="s">
         <v>9</v>
       </c>
@@ -1951,7 +2085,7 @@
         <v>1.0498000000000047</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
         <v>10</v>
       </c>
@@ -1990,7 +2124,7 @@
         <v>12.837400000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18">
       <c r="A25" s="8" t="s">
         <v>12</v>
       </c>
@@ -2029,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18">
       <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
@@ -2068,9 +2202,9 @@
         <v>13.757500000000022</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18">
       <c r="A27" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" s="8">
         <v>2</v>
@@ -2088,7 +2222,7 @@
         <v>162.93430000000001</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H27" s="8">
         <f t="shared" si="3"/>
@@ -2107,7 +2241,7 @@
         <v>15.892600000000016</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -2120,7 +2254,7 @@
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18">
       <c r="A29" s="8" t="s">
         <v>14</v>
       </c>
@@ -2147,7 +2281,7 @@
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18">
       <c r="F30" s="9"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -2155,383 +2289,277 @@
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18">
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18">
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:8">
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:8">
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C35" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D35" s="10">
-        <v>147.2595</v>
-      </c>
-      <c r="E35" s="10">
-        <v>147.2595</v>
-      </c>
-      <c r="F35" s="10">
-        <v>147.2595</v>
-      </c>
-      <c r="G35" s="10">
-        <v>147.2595</v>
-      </c>
+    <row r="35" spans="3:8">
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C36" s="10">
-        <v>2</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E36" s="10">
-        <v>133.4178</v>
-      </c>
-      <c r="F36" s="10">
-        <v>142.3364</v>
-      </c>
-      <c r="G36" s="10">
-        <v>144.1619</v>
-      </c>
-      <c r="H36" s="10">
-        <v>160.45660000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C37" s="10">
-        <v>3</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="10">
-        <v>132.1293</v>
-      </c>
-      <c r="F37" s="10">
-        <v>141.5848</v>
-      </c>
-      <c r="G37" s="10">
-        <v>148.9504</v>
-      </c>
-      <c r="H37" s="10">
-        <v>159.74369999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C38" s="10">
-        <v>4</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E38" s="10">
-        <v>134.92619999999999</v>
-      </c>
-      <c r="F38" s="10">
-        <v>143.77529999999999</v>
-      </c>
-      <c r="G38" s="10">
-        <v>148.04220000000001</v>
-      </c>
-      <c r="H38" s="10">
-        <v>160.1679</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C39" s="10">
-        <v>5</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="E39" s="10">
-        <v>135.08459999999999</v>
-      </c>
-      <c r="F39" s="10">
-        <v>143.94630000000001</v>
-      </c>
-      <c r="G39" s="10">
-        <v>147.67420000000001</v>
-      </c>
-      <c r="H39" s="10">
-        <v>148.0915</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C40" s="10">
-        <v>6</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="E40" s="10">
-        <v>133.23820000000001</v>
-      </c>
-      <c r="F40" s="10">
-        <v>142.4992</v>
-      </c>
-      <c r="G40" s="10">
-        <v>148.98570000000001</v>
-      </c>
-      <c r="H40" s="10">
-        <v>159.87909999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C41" s="10">
-        <v>7</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="10">
-        <v>137.98169999999999</v>
-      </c>
-      <c r="F41" s="10">
-        <v>146.83019999999999</v>
-      </c>
-      <c r="G41" s="10">
-        <v>150.06059999999999</v>
-      </c>
-      <c r="H41" s="10">
-        <v>147.04169999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C42" s="10">
-        <v>8</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E42" s="10">
-        <v>133.1848</v>
-      </c>
-      <c r="F42" s="10">
-        <v>142.6403</v>
-      </c>
-      <c r="G42" s="10">
-        <v>150.006</v>
-      </c>
-      <c r="H42" s="10">
-        <v>160.79920000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C43" s="10">
-        <v>9</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="10">
-        <v>134.2484</v>
-      </c>
-      <c r="F43" s="10">
-        <v>143.65270000000001</v>
-      </c>
-      <c r="G43" s="10">
-        <v>147.2141</v>
-      </c>
-      <c r="H43" s="10">
-        <v>162.93430000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:8">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="3:8">
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="3:8">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="3:8">
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="3:8">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="3:8">
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="3:8">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="3:8">
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="3:8">
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:8">
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:8">
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:8">
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:8">
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="7:7">
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="7:7">
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="7:7">
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="7:7">
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="7:7">
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="7:7">
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="7:7">
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="7:7">
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="7:7">
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="7:7">
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="7:7">
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="7:7">
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="7:7">
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="7:7">
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="7:7">
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="7:7">
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="7:7">
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="7:7">
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="7:7">
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="7:7">
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="7:7">
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="7:7">
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="7:7">
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="7:7">
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="7:7">
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="7:7">
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="7:7">
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="7:7">
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="7:7">
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="7:7">
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="7:7">
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="7:7">
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="7:7">
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="7:7">
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="7:7">
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="7:7">
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="7:7">
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="7:7">
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="7:7">
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="7:7">
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="7:7">
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="7:7">
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="7:7">
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="7:7">
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="7:7">
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="7:7">
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="7:7">
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="7:7">
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="7:7">
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="7:7">
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="7:7">
       <c r="G99" s="6"/>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="7:7">
       <c r="G100" s="6"/>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="7:7">
       <c r="G101" s="6"/>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="7:7">
       <c r="G102" s="6"/>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="7:7">
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="7:7">
       <c r="G104" s="6"/>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="7:7">
       <c r="G105" s="6"/>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="7:7">
       <c r="G106" s="6"/>
     </row>
   </sheetData>
@@ -2553,46 +2581,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB75A54-5B89-9C4C-94E4-40B803093B20}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:E41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10" style="31" customWidth="1"/>
     <col min="2" max="2" width="26" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="31"/>
-    <col min="6" max="6" width="11.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="31"/>
+    <col min="3" max="3" width="12.625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.875" style="31"/>
+    <col min="6" max="6" width="11.625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="31.5">
       <c r="A1" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="51" t="s">
         <v>165</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
-        <v>166</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>150</v>
@@ -2616,8 +2644,8 @@
       </c>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="47"/>
+    <row r="3" spans="1:16">
+      <c r="A3" s="51"/>
       <c r="B3" s="33" t="s">
         <v>7</v>
       </c>
@@ -2640,8 +2668,8 @@
       </c>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
+    <row r="4" spans="1:16">
+      <c r="A4" s="51"/>
       <c r="B4" s="33" t="s">
         <v>148</v>
       </c>
@@ -2669,13 +2697,13 @@
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
     </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
+    <row r="5" spans="1:16">
+      <c r="A5" s="51"/>
       <c r="B5" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>171</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>172</v>
       </c>
       <c r="D5" s="33">
         <v>44.726619999999997</v>
@@ -2699,13 +2727,13 @@
       <c r="O5" s="10"/>
       <c r="P5" s="17"/>
     </row>
-    <row r="6" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A6" s="51"/>
       <c r="B6" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" s="34">
         <v>46.135950000000001</v>
@@ -2729,8 +2757,8 @@
       <c r="O6" s="10"/>
       <c r="P6" s="17"/>
     </row>
-    <row r="7" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+    <row r="7" spans="1:16" ht="16.5" thickTop="1">
+      <c r="A7" s="51"/>
       <c r="B7" s="33" t="s">
         <v>149</v>
       </c>
@@ -2760,10 +2788,10 @@
       <c r="O7" s="10"/>
       <c r="P7" s="17"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+    <row r="8" spans="1:16">
+      <c r="A8" s="51"/>
       <c r="B8" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="36">
         <v>0.98499999999999999</v>
@@ -2791,13 +2819,13 @@
       <c r="O8" s="10"/>
       <c r="P8" s="17"/>
     </row>
-    <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+    <row r="9" spans="1:16" ht="31.5">
+      <c r="A9" s="51"/>
       <c r="B9" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>175</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>176</v>
       </c>
       <c r="D9" s="33">
         <v>47.806550000000001</v>
@@ -2821,13 +2849,13 @@
       <c r="O9" s="10"/>
       <c r="P9" s="17"/>
     </row>
-    <row r="10" spans="1:16" ht="85" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
+    <row r="10" spans="1:16" ht="78.75">
+      <c r="A10" s="51"/>
       <c r="B10" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" s="33">
         <v>53.080280000000002</v>
@@ -2852,9 +2880,9 @@
       <c r="O10" s="10"/>
       <c r="P10" s="17"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
-        <v>167</v>
+    <row r="11" spans="1:16">
+      <c r="A11" s="51" t="s">
+        <v>166</v>
       </c>
       <c r="B11" s="37" t="s">
         <v>7</v>
@@ -2885,8 +2913,8 @@
       <c r="O11" s="10"/>
       <c r="P11" s="17"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
+    <row r="12" spans="1:16">
+      <c r="A12" s="51"/>
       <c r="B12" s="37" t="s">
         <v>150</v>
       </c>
@@ -2916,13 +2944,13 @@
       <c r="O12" s="10"/>
       <c r="P12" s="17"/>
     </row>
-    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
+    <row r="13" spans="1:16">
+      <c r="A13" s="51"/>
       <c r="B13" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>171</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>172</v>
       </c>
       <c r="D13" s="37">
         <v>45.299619999999997</v>
@@ -2948,8 +2976,8 @@
       <c r="O13" s="10"/>
       <c r="P13" s="17"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
+    <row r="14" spans="1:16">
+      <c r="A14" s="51"/>
       <c r="B14" s="37" t="s">
         <v>148</v>
       </c>
@@ -2979,8 +3007,8 @@
       <c r="O14" s="10"/>
       <c r="P14" s="17"/>
     </row>
-    <row r="15" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+    <row r="15" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A15" s="51"/>
       <c r="B15" s="37" t="s">
         <v>149</v>
       </c>
@@ -3009,13 +3037,13 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
     </row>
-    <row r="16" spans="1:16" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
+    <row r="16" spans="1:16" ht="32.25" thickTop="1">
+      <c r="A16" s="51"/>
       <c r="B16" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D16" s="37">
         <v>47.765250000000002</v>
@@ -3040,10 +3068,10 @@
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="47"/>
+    <row r="17" spans="1:11">
+      <c r="A17" s="51"/>
       <c r="B17" s="37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C17" s="31">
         <v>0.9073</v>
@@ -3067,13 +3095,13 @@
       <c r="J17" s="10"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
+    <row r="18" spans="1:11" ht="31.5">
+      <c r="A18" s="51"/>
       <c r="B18" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D18" s="37">
         <v>48.809289999999997</v>
@@ -3094,13 +3122,13 @@
       <c r="J18" s="10"/>
       <c r="K18" s="19"/>
     </row>
-    <row r="19" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
+    <row r="19" spans="1:11" ht="78.75">
+      <c r="A19" s="51"/>
       <c r="B19" s="37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="37">
         <v>61.65701</v>
@@ -3121,8 +3149,8 @@
       <c r="J19" s="10"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:11">
+      <c r="A20" s="51" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="33" t="s">
@@ -3135,7 +3163,7 @@
         <v>41.431260000000002</v>
       </c>
       <c r="E20" s="32">
-        <f t="shared" ref="E20:E41" si="1">D20-MIN($D$2:$D$11)</f>
+        <f t="shared" ref="E20:E30" si="1">D20-MIN($D$2:$D$11)</f>
         <v>-1.2904199999999975</v>
       </c>
       <c r="F20" s="40">
@@ -3150,8 +3178,8 @@
       <c r="J20" s="10"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="47"/>
+    <row r="21" spans="1:11">
+      <c r="A21" s="51"/>
       <c r="B21" s="33" t="s">
         <v>7</v>
       </c>
@@ -3177,13 +3205,13 @@
       <c r="J21" s="10"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="47"/>
+    <row r="22" spans="1:11">
+      <c r="A22" s="51"/>
       <c r="B22" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>171</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>172</v>
       </c>
       <c r="D22" s="33">
         <v>43.183140000000002</v>
@@ -3204,8 +3232,8 @@
       <c r="J22" s="10"/>
       <c r="K22" s="19"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="47"/>
+    <row r="23" spans="1:11">
+      <c r="A23" s="51"/>
       <c r="B23" s="33" t="s">
         <v>148</v>
       </c>
@@ -3231,13 +3259,13 @@
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="47"/>
+    <row r="24" spans="1:11" ht="31.5">
+      <c r="A24" s="51"/>
       <c r="B24" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D24" s="33">
         <v>44.954700000000003</v>
@@ -3258,8 +3286,8 @@
       <c r="J24" s="10"/>
       <c r="K24" s="18"/>
     </row>
-    <row r="25" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+    <row r="25" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A25" s="51"/>
       <c r="B25" s="34" t="s">
         <v>149</v>
       </c>
@@ -3285,10 +3313,10 @@
       <c r="J25" s="10"/>
       <c r="K25" s="18"/>
     </row>
-    <row r="26" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="47"/>
+    <row r="26" spans="1:11" ht="16.5" thickTop="1">
+      <c r="A26" s="51"/>
       <c r="B26" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" s="36">
         <v>0.89800000000000002</v>
@@ -3311,10 +3339,10 @@
       <c r="I26" s="19"/>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="47"/>
+    <row r="27" spans="1:11">
+      <c r="A27" s="51"/>
       <c r="B27" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" s="36">
         <v>0.91</v>
@@ -3337,13 +3365,13 @@
       <c r="I27" s="18"/>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="47"/>
+    <row r="28" spans="1:11" ht="31.5">
+      <c r="A28" s="51"/>
       <c r="B28" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D28" s="33">
         <v>46.423520000000003</v>
@@ -3363,13 +3391,13 @@
       <c r="I28" s="18"/>
       <c r="K28" s="18"/>
     </row>
-    <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="47"/>
+    <row r="29" spans="1:11" ht="31.5">
+      <c r="A29" s="51"/>
       <c r="B29" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>185</v>
       </c>
       <c r="D29" s="33">
         <v>47.297080000000001</v>
@@ -3389,13 +3417,13 @@
       <c r="I29" s="18"/>
       <c r="K29" s="18"/>
     </row>
-    <row r="30" spans="1:11" ht="102" x14ac:dyDescent="0.2">
-      <c r="A30" s="47"/>
+    <row r="30" spans="1:11" ht="94.5">
+      <c r="A30" s="51"/>
       <c r="B30" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C30" s="32" t="s">
         <v>186</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>187</v>
       </c>
       <c r="D30" s="33">
         <v>57.785269999999997</v>
@@ -3415,15 +3443,15 @@
       <c r="I30" s="19"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="47" t="s">
+    <row r="31" spans="1:11">
+      <c r="A31" s="51" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" s="32" t="s">
         <v>171</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>172</v>
       </c>
       <c r="D31" s="33">
         <v>55.85942</v>
@@ -3443,10 +3471,10 @@
       <c r="I31" s="18"/>
       <c r="K31" s="18"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="47"/>
+    <row r="32" spans="1:11">
+      <c r="A32" s="51"/>
       <c r="B32" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C32" s="32">
         <v>0.35099999999999998</v>
@@ -3469,8 +3497,8 @@
       <c r="I32" s="18"/>
       <c r="K32" s="18"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="47"/>
+    <row r="33" spans="1:11">
+      <c r="A33" s="51"/>
       <c r="B33" s="33" t="s">
         <v>7</v>
       </c>
@@ -3495,8 +3523,8 @@
       <c r="I33" s="18"/>
       <c r="K33" s="18"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="47"/>
+    <row r="34" spans="1:11">
+      <c r="A34" s="51"/>
       <c r="B34" s="33" t="s">
         <v>149</v>
       </c>
@@ -3521,8 +3549,8 @@
       <c r="I34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="47"/>
+    <row r="35" spans="1:11">
+      <c r="A35" s="51"/>
       <c r="B35" s="33" t="s">
         <v>150</v>
       </c>
@@ -3547,10 +3575,10 @@
       <c r="I35" s="18"/>
       <c r="K35" s="18"/>
     </row>
-    <row r="36" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+    <row r="36" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A36" s="51"/>
       <c r="B36" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C36" s="35">
         <v>0.749</v>
@@ -3573,8 +3601,8 @@
       <c r="I36" s="18"/>
       <c r="K36" s="18"/>
     </row>
-    <row r="37" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="47"/>
+    <row r="37" spans="1:11" ht="16.5" thickTop="1">
+      <c r="A37" s="51"/>
       <c r="B37" s="33" t="s">
         <v>148</v>
       </c>
@@ -3599,13 +3627,13 @@
       <c r="I37" s="18"/>
       <c r="K37" s="18"/>
     </row>
-    <row r="38" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="47"/>
+    <row r="38" spans="1:11" ht="31.5">
+      <c r="A38" s="51"/>
       <c r="B38" s="33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D38" s="33">
         <v>61.300179999999997</v>
@@ -3625,13 +3653,13 @@
       <c r="I38" s="19"/>
       <c r="K38" s="19"/>
     </row>
-    <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="47"/>
+    <row r="39" spans="1:11">
+      <c r="A39" s="51"/>
       <c r="B39" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D39" s="33">
         <v>61.951509999999999</v>
@@ -3650,13 +3678,13 @@
       <c r="H39" s="18"/>
       <c r="K39" s="18"/>
     </row>
-    <row r="40" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="47"/>
+    <row r="40" spans="1:11" ht="31.5">
+      <c r="A40" s="51"/>
       <c r="B40" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D40" s="33">
         <v>62.24259</v>
@@ -3675,13 +3703,13 @@
       <c r="H40" s="18"/>
       <c r="K40" s="18"/>
     </row>
-    <row r="41" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A41" s="47"/>
+    <row r="41" spans="1:11" ht="78.75">
+      <c r="A41" s="51"/>
       <c r="B41" s="37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D41" s="33">
         <v>91.646410000000003</v>
@@ -3700,66 +3728,66 @@
       <c r="H41" s="18"/>
       <c r="K41" s="18"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="C42" s="44"/>
       <c r="D42" s="44"/>
       <c r="H42" s="19"/>
       <c r="K42" s="19"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="C43" s="44"/>
       <c r="D43" s="44"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="C44" s="44"/>
       <c r="D44" s="44"/>
       <c r="H44" s="18"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="C45" s="44"/>
       <c r="D45" s="44"/>
       <c r="H45" s="18"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="C46" s="44"/>
       <c r="D46" s="44"/>
       <c r="H46" s="19"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="C47" s="44"/>
       <c r="D47" s="44"/>
       <c r="H47" s="18"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="C48" s="44"/>
       <c r="H48" s="18"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:8">
       <c r="C49" s="44"/>
       <c r="H49" s="18"/>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:8">
       <c r="C50" s="44"/>
       <c r="H50" s="19"/>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:8">
       <c r="C51" s="44"/>
       <c r="H51" s="18"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:8">
       <c r="C52" s="44"/>
       <c r="H52" s="18"/>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:8">
       <c r="C53" s="44"/>
       <c r="H53" s="18"/>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:8">
       <c r="C54" s="44"/>
       <c r="H54" s="19"/>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:8">
       <c r="C55" s="44"/>
     </row>
   </sheetData>
@@ -3786,111 +3814,111 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="31.5">
       <c r="A1" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>164</v>
-      </c>
       <c r="F1" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I1" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="32" t="s">
-        <v>164</v>
-      </c>
       <c r="N1" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q1" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="R1" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="S1" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="T1" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="U1" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="32" t="s">
-        <v>164</v>
-      </c>
       <c r="V1" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="W1" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Y1" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z1" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="AA1" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="AA1" s="32" t="s">
+      <c r="AB1" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="AB1" s="32" t="s">
+      <c r="AC1" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="AC1" s="32" t="s">
-        <v>164</v>
-      </c>
       <c r="AD1" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AE1" s="32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
-        <v>166</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="15.95" customHeight="1">
+      <c r="A2" s="51" t="s">
+        <v>165</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>7</v>
@@ -3902,7 +3930,7 @@
         <v>132.1293</v>
       </c>
       <c r="E2" s="32">
-        <f>D2-MIN($D$2:$D$10)</f>
+        <f t="shared" ref="E2:E10" si="0">D2-MIN($D$2:$D$10)</f>
         <v>0</v>
       </c>
       <c r="F2" s="10">
@@ -3912,8 +3940,8 @@
         <f>SUM(F1:F2)</f>
         <v>0.27825261019999997</v>
       </c>
-      <c r="I2" s="47" t="s">
-        <v>167</v>
+      <c r="I2" s="51" t="s">
+        <v>166</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>7</v>
@@ -3925,7 +3953,7 @@
         <v>141.5848</v>
       </c>
       <c r="M2" s="32">
-        <f>L2-MIN($L$2:$L$10)</f>
+        <f t="shared" ref="M2:M10" si="1">L2-MIN($L$2:$L$10)</f>
         <v>0</v>
       </c>
       <c r="N2" s="26">
@@ -3935,7 +3963,7 @@
         <f>SUM(N1:N2)</f>
         <v>0.23696529999999999</v>
       </c>
-      <c r="Q2" s="47" t="s">
+      <c r="Q2" s="51" t="s">
         <v>2</v>
       </c>
       <c r="R2" s="10" t="s">
@@ -3948,30 +3976,30 @@
         <v>144.1619</v>
       </c>
       <c r="U2" s="32">
-        <f>T2-MIN($T$2:$T$10)</f>
+        <f t="shared" ref="U2:U10" si="2">T2-MIN($T$2:$T$10)</f>
         <v>0</v>
       </c>
-      <c r="V2" s="51">
+      <c r="V2" s="49">
         <v>0.49733889999999997</v>
       </c>
       <c r="W2" s="32">
         <f>SUM(V1:V2)</f>
         <v>0.49733889999999997</v>
       </c>
-      <c r="Y2" s="47" t="s">
+      <c r="Y2" s="51" t="s">
         <v>3</v>
       </c>
       <c r="Z2" s="10" t="s">
         <v>151</v>
       </c>
       <c r="AA2" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB2" s="10">
         <v>147.04169999999999</v>
       </c>
       <c r="AC2" s="32">
-        <f>AB2-MIN($AB$2:$AB$10)</f>
+        <f t="shared" ref="AC2:AC10" si="3">AB2-MIN($AB$2:$AB$10)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="10">
@@ -3982,17 +4010,17 @@
         <v>0.62388120400000002</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" s="47"/>
+    <row r="3" spans="1:31">
+      <c r="A3" s="51"/>
       <c r="B3" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="10">
         <v>133.09</v>
       </c>
       <c r="E3" s="32">
-        <f>D3-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>0.96070000000000277</v>
       </c>
       <c r="F3" s="10">
@@ -4002,16 +4030,16 @@
         <f>SUM(F1:F3)</f>
         <v>0.45037073789999998</v>
       </c>
-      <c r="I3" s="47"/>
+      <c r="I3" s="51"/>
       <c r="J3" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="10">
         <v>141.9571</v>
       </c>
       <c r="M3" s="32">
-        <f>L3-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>0.37229999999999563</v>
       </c>
       <c r="N3" s="26">
@@ -4021,26 +4049,26 @@
         <f>SUM(N2:N3)</f>
         <v>0.4336834</v>
       </c>
-      <c r="Q3" s="47"/>
+      <c r="Q3" s="51"/>
       <c r="R3" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S3" s="32"/>
       <c r="T3" s="10">
         <v>146.98660000000001</v>
       </c>
       <c r="U3" s="32">
-        <f>T3-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>2.8247000000000071</v>
       </c>
-      <c r="V3" s="51">
+      <c r="V3" s="49">
         <v>0.1211348</v>
       </c>
       <c r="W3" s="32">
         <f>SUM(V1:V3)</f>
         <v>0.61847370000000002</v>
       </c>
-      <c r="Y3" s="47"/>
+      <c r="Y3" s="51"/>
       <c r="Z3" s="10" t="s">
         <v>150</v>
       </c>
@@ -4051,7 +4079,7 @@
         <v>148.0915</v>
       </c>
       <c r="AC3" s="32">
-        <f>AB3-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>1.0498000000000047</v>
       </c>
       <c r="AD3" s="10">
@@ -4062,10 +4090,10 @@
         <v>0.99297676079999997</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
+    <row r="4" spans="1:31" ht="31.5">
+      <c r="A4" s="51"/>
       <c r="B4" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="36">
         <v>0.23100000000000001</v>
@@ -4074,7 +4102,7 @@
         <v>133.23820000000001</v>
       </c>
       <c r="E4" s="32">
-        <f>D4-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>1.1089000000000055</v>
       </c>
       <c r="F4" s="10">
@@ -4084,7 +4112,7 @@
         <f>SUM(F1:F4)</f>
         <v>0.61019451589999996</v>
       </c>
-      <c r="I4" s="47"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="10" t="s">
         <v>148</v>
       </c>
@@ -4095,7 +4123,7 @@
         <v>142.3364</v>
       </c>
       <c r="M4" s="32">
-        <f>L4-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>0.75159999999999627</v>
       </c>
       <c r="N4" s="26">
@@ -4105,37 +4133,37 @@
         <f>SUM(N2:N4)</f>
         <v>0.59641500000000003</v>
       </c>
-      <c r="Q4" s="47"/>
+      <c r="Q4" s="51"/>
       <c r="R4" s="10" t="s">
         <v>152</v>
       </c>
       <c r="S4" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T4" s="10">
         <v>147.2141</v>
       </c>
       <c r="U4" s="32">
-        <f>T4-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>3.0521999999999991</v>
       </c>
-      <c r="V4" s="51">
+      <c r="V4" s="49">
         <v>0.1081119</v>
       </c>
       <c r="W4" s="32">
         <f>SUM(V1:V4)</f>
         <v>0.72658560000000005</v>
       </c>
-      <c r="Y4" s="47"/>
+      <c r="Y4" s="51"/>
       <c r="Z4" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AA4" s="32"/>
       <c r="AB4" s="10">
         <v>158.45679999999999</v>
       </c>
       <c r="AC4" s="32">
-        <f>AB4-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>11.415099999999995</v>
       </c>
       <c r="AD4" s="10">
@@ -4146,8 +4174,8 @@
         <v>0.995048559</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
+    <row r="5" spans="1:31">
+      <c r="A5" s="51"/>
       <c r="B5" s="10" t="s">
         <v>148</v>
       </c>
@@ -4158,7 +4186,7 @@
         <v>133.4178</v>
       </c>
       <c r="E5" s="32">
-        <f>D5-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>1.2884999999999991</v>
       </c>
       <c r="F5" s="10">
@@ -4168,9 +4196,9 @@
         <f>SUM(F2:F5)</f>
         <v>0.7562878972</v>
       </c>
-      <c r="I5" s="47"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K5" s="32">
         <v>0.28799999999999998</v>
@@ -4179,7 +4207,7 @@
         <v>142.4992</v>
       </c>
       <c r="M5" s="32">
-        <f>L5-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>0.91440000000000055</v>
       </c>
       <c r="N5" s="26">
@@ -4189,7 +4217,7 @@
         <f>SUM(N2:N5)</f>
         <v>0.74642450000000005</v>
       </c>
-      <c r="Q5" s="47"/>
+      <c r="Q5" s="51"/>
       <c r="R5" s="10" t="s">
         <v>150</v>
       </c>
@@ -4200,17 +4228,17 @@
         <v>147.67420000000001</v>
       </c>
       <c r="U5" s="32">
-        <f>T5-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>3.5123000000000104</v>
       </c>
-      <c r="V5" s="51">
+      <c r="V5" s="49">
         <v>8.5895429999999995E-2</v>
       </c>
       <c r="W5" s="32">
         <f>SUM(V1:V5)</f>
         <v>0.81248103000000005</v>
       </c>
-      <c r="Y5" s="47"/>
+      <c r="Y5" s="51"/>
       <c r="Z5" s="10" t="s">
         <v>7</v>
       </c>
@@ -4221,7 +4249,7 @@
         <v>159.74369999999999</v>
       </c>
       <c r="AC5" s="32">
-        <f>AB5-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>12.701999999999998</v>
       </c>
       <c r="AD5" s="10">
@@ -4232,19 +4260,19 @@
         <v>0.99613724439999995</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+    <row r="6" spans="1:31" ht="31.5">
+      <c r="A6" s="51"/>
       <c r="B6" s="10" t="s">
         <v>152</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" s="10">
         <v>134.2484</v>
       </c>
       <c r="E6" s="32">
-        <f>D6-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>2.1191000000000031</v>
       </c>
       <c r="F6" s="10">
@@ -4254,18 +4282,18 @@
         <f>SUM(F1:F6)</f>
         <v>0.85273060590000005</v>
       </c>
-      <c r="I6" s="47"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="10" t="s">
         <v>152</v>
       </c>
       <c r="K6" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L6" s="10">
         <v>143.65270000000001</v>
       </c>
       <c r="M6" s="32">
-        <f>L6-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>2.0679000000000087</v>
       </c>
       <c r="N6" s="26">
@@ -4275,7 +4303,7 @@
         <f>SUM(N2:N6)</f>
         <v>0.83068685000000009</v>
       </c>
-      <c r="Q6" s="47"/>
+      <c r="Q6" s="51"/>
       <c r="R6" s="10" t="s">
         <v>149</v>
       </c>
@@ -4286,19 +4314,19 @@
         <v>148.04220000000001</v>
       </c>
       <c r="U6" s="32">
-        <f>T6-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>3.8803000000000054</v>
       </c>
-      <c r="V6" s="51">
+      <c r="V6" s="49">
         <v>7.1458199999999999E-2</v>
       </c>
       <c r="W6" s="32">
         <f>SUM(V1:V6)</f>
         <v>0.88393923000000008</v>
       </c>
-      <c r="Y6" s="47"/>
+      <c r="Y6" s="51"/>
       <c r="Z6" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA6" s="32">
         <v>0.504</v>
@@ -4307,7 +4335,7 @@
         <v>159.87909999999999</v>
       </c>
       <c r="AC6" s="32">
-        <f>AB6-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>12.837400000000002</v>
       </c>
       <c r="AD6" s="10">
@@ -4318,8 +4346,8 @@
         <v>0.99715466149999998</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+    <row r="7" spans="1:31" ht="78.75">
+      <c r="A7" s="51"/>
       <c r="B7" s="10" t="s">
         <v>149</v>
       </c>
@@ -4330,7 +4358,7 @@
         <v>134.92619999999999</v>
       </c>
       <c r="E7" s="32">
-        <f>D7-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>2.7968999999999937</v>
       </c>
       <c r="F7" s="10">
@@ -4340,7 +4368,7 @@
         <f>SUM(F2:F7)</f>
         <v>0.92145336320000004</v>
       </c>
-      <c r="I7" s="47"/>
+      <c r="I7" s="51"/>
       <c r="J7" s="10" t="s">
         <v>149</v>
       </c>
@@ -4351,7 +4379,7 @@
         <v>143.77529999999999</v>
       </c>
       <c r="M7" s="32">
-        <f>L7-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>2.1904999999999859</v>
       </c>
       <c r="N7" s="26">
@@ -4361,7 +4389,7 @@
         <f>SUM(N2:N7)</f>
         <v>0.90993956000000009</v>
       </c>
-      <c r="Q7" s="47"/>
+      <c r="Q7" s="51"/>
       <c r="R7" s="10" t="s">
         <v>7</v>
       </c>
@@ -4372,28 +4400,28 @@
         <v>148.9504</v>
       </c>
       <c r="U7" s="32">
-        <f>T7-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>4.7884999999999991</v>
       </c>
-      <c r="V7" s="51">
+      <c r="V7" s="49">
         <v>4.5377189999999998E-2</v>
       </c>
       <c r="W7" s="32">
         <f>SUM(V1:V7)</f>
         <v>0.92931642000000003</v>
       </c>
-      <c r="Y7" s="47"/>
+      <c r="Y7" s="51"/>
       <c r="Z7" s="10" t="s">
         <v>147</v>
       </c>
       <c r="AA7" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB7" s="10">
         <v>159.95050000000001</v>
       </c>
       <c r="AC7" s="32">
-        <f>AB7-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>12.908800000000014</v>
       </c>
       <c r="AD7" s="10">
@@ -4404,8 +4432,8 @@
         <v>1.9991158000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+    <row r="8" spans="1:31">
+      <c r="A8" s="51"/>
       <c r="B8" s="10" t="s">
         <v>150</v>
       </c>
@@ -4416,7 +4444,7 @@
         <v>135.08459999999999</v>
       </c>
       <c r="E8" s="32">
-        <f>D8-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>2.955299999999994</v>
       </c>
       <c r="F8" s="10">
@@ -4426,7 +4454,7 @@
         <f>SUM(F2:F8)</f>
         <v>0.984941756</v>
       </c>
-      <c r="I8" s="47"/>
+      <c r="I8" s="51"/>
       <c r="J8" s="10" t="s">
         <v>150</v>
       </c>
@@ -4437,7 +4465,7 @@
         <v>143.94630000000001</v>
       </c>
       <c r="M8" s="32">
-        <f>L8-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>2.3615000000000066</v>
       </c>
       <c r="N8" s="26">
@@ -4447,9 +4475,9 @@
         <f>SUM(N2:N8)</f>
         <v>0.98269951000000011</v>
       </c>
-      <c r="Q8" s="47"/>
+      <c r="Q8" s="51"/>
       <c r="R8" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S8" s="32">
         <v>0.97799999999999998</v>
@@ -4458,17 +4486,17 @@
         <v>148.98570000000001</v>
       </c>
       <c r="U8" s="32">
-        <f>T8-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>4.8238000000000056</v>
       </c>
-      <c r="V8" s="51">
+      <c r="V8" s="49">
         <v>4.4584110000000003E-2</v>
       </c>
       <c r="W8" s="32">
         <f>SUM(V1:V8)</f>
         <v>0.97390052999999999</v>
       </c>
-      <c r="Y8" s="47"/>
+      <c r="Y8" s="51"/>
       <c r="Z8" s="10" t="s">
         <v>149</v>
       </c>
@@ -4479,7 +4507,7 @@
         <v>160.1679</v>
       </c>
       <c r="AC8" s="32">
-        <f>AB8-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>13.126200000000011</v>
       </c>
       <c r="AD8" s="10">
@@ -4490,19 +4518,19 @@
         <v>0.99901695329999995</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+    <row r="9" spans="1:31" ht="31.5">
+      <c r="A9" s="51"/>
       <c r="B9" s="10" t="s">
         <v>151</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D9" s="10">
         <v>137.98169999999999</v>
       </c>
       <c r="E9" s="32">
-        <f>D9-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>5.8523999999999887</v>
       </c>
       <c r="F9" s="10">
@@ -4512,18 +4540,18 @@
         <f>SUM(F2:F9)</f>
         <v>0.99985580269999996</v>
       </c>
-      <c r="I9" s="47"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="10" t="s">
         <v>151</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L9" s="10">
         <v>146.83019999999999</v>
       </c>
       <c r="M9" s="32">
-        <f>L9-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>5.2453999999999894</v>
       </c>
       <c r="N9" s="26">
@@ -4533,28 +4561,28 @@
         <f>SUM(N2:N9)</f>
         <v>0.99990460000000014</v>
       </c>
-      <c r="Q9" s="47"/>
+      <c r="Q9" s="51"/>
       <c r="R9" s="10" t="s">
         <v>151</v>
       </c>
       <c r="S9" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="T9" s="10">
         <v>150.06059999999999</v>
       </c>
       <c r="U9" s="32">
-        <f>T9-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>5.898699999999991</v>
       </c>
-      <c r="V9" s="51">
+      <c r="V9" s="49">
         <v>2.604654E-2</v>
       </c>
       <c r="W9" s="32">
         <f>SUM(V1:V9)</f>
         <v>0.99994706999999994</v>
       </c>
-      <c r="Y9" s="47"/>
+      <c r="Y9" s="51"/>
       <c r="Z9" s="10" t="s">
         <v>148</v>
       </c>
@@ -4565,7 +4593,7 @@
         <v>160.45660000000001</v>
       </c>
       <c r="AC9" s="32">
-        <f>AB9-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>13.414900000000017</v>
       </c>
       <c r="AD9" s="10">
@@ -4576,19 +4604,19 @@
         <v>0.99977916999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="85" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
+    <row r="10" spans="1:31" ht="78.75">
+      <c r="A10" s="51"/>
       <c r="B10" s="10" t="s">
         <v>147</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D10" s="10">
         <v>147.2595</v>
       </c>
       <c r="E10" s="32">
-        <f>D10-MIN($D$2:$D$10)</f>
+        <f t="shared" si="0"/>
         <v>15.130200000000002</v>
       </c>
       <c r="F10" s="10">
@@ -4598,18 +4626,18 @@
         <f>SUM(F2:F10)</f>
         <v>1</v>
       </c>
-      <c r="I10" s="47"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="10" t="s">
         <v>147</v>
       </c>
       <c r="K10" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="L10" s="50">
+        <v>204</v>
+      </c>
+      <c r="L10" s="48">
         <v>157.22069999999999</v>
       </c>
       <c r="M10" s="32">
-        <f>L10-MIN($L$2:$L$10)</f>
+        <f t="shared" si="1"/>
         <v>15.635899999999992</v>
       </c>
       <c r="N10" s="26">
@@ -4619,39 +4647,39 @@
         <f>SUM(N2:N10)</f>
         <v>0.99999996458000018</v>
       </c>
-      <c r="Q10" s="47"/>
+      <c r="Q10" s="51"/>
       <c r="R10" s="10" t="s">
         <v>147</v>
       </c>
       <c r="S10" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="T10" s="10">
         <v>162.46119999999999</v>
       </c>
       <c r="U10" s="32">
-        <f>T10-MIN($T$2:$T$10)</f>
+        <f t="shared" si="2"/>
         <v>18.299299999999988</v>
       </c>
-      <c r="V10" s="51">
+      <c r="V10" s="49">
         <v>5.2844979999999998E-5</v>
       </c>
       <c r="W10" s="32">
         <f>SUM(V7:V10)</f>
         <v>0.11606068498</v>
       </c>
-      <c r="Y10" s="47"/>
+      <c r="Y10" s="51"/>
       <c r="Z10" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AA10" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB10" s="10">
         <v>162.93430000000001</v>
       </c>
       <c r="AC10" s="32">
-        <f>AB10-MIN($AB$2:$AB$10)</f>
+        <f t="shared" si="3"/>
         <v>15.892600000000016</v>
       </c>
       <c r="AD10" s="10">
@@ -4662,7 +4690,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31">
       <c r="A11" s="31"/>
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
@@ -4674,8 +4702,8 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
+    <row r="12" spans="1:31" ht="15.95" customHeight="1">
+      <c r="A12" s="51"/>
       <c r="B12" s="10"/>
       <c r="C12" s="32"/>
       <c r="D12" s="10"/>
@@ -4686,8 +4714,8 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
+    <row r="13" spans="1:31">
+      <c r="A13" s="51"/>
       <c r="B13" s="10"/>
       <c r="C13" s="32"/>
       <c r="D13" s="10"/>
@@ -4698,8 +4726,8 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
+    <row r="14" spans="1:31">
+      <c r="A14" s="51"/>
       <c r="B14" s="10"/>
       <c r="C14" s="32"/>
       <c r="D14" s="10"/>
@@ -4714,17 +4742,17 @@
       <c r="U14" s="10"/>
       <c r="V14" s="13"/>
       <c r="AB14" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC14" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD14" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="AD14" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" s="51"/>
       <c r="B15" s="10"/>
       <c r="C15" s="32"/>
       <c r="D15" s="10"/>
@@ -4735,13 +4763,13 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M15" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="N15" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -4752,8 +4780,8 @@
       <c r="AD15" s="9"/>
       <c r="AE15" s="9"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
+    <row r="16" spans="1:31">
+      <c r="A16" s="51"/>
       <c r="B16" s="10"/>
       <c r="C16" s="32"/>
       <c r="D16" s="10"/>
@@ -4778,8 +4806,8 @@
       <c r="AD16" s="10"/>
       <c r="AE16" s="10"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="47"/>
+    <row r="17" spans="1:31">
+      <c r="A17" s="51"/>
       <c r="B17" s="10"/>
       <c r="C17" s="32"/>
       <c r="D17" s="10"/>
@@ -4803,8 +4831,8 @@
       <c r="AD17" s="10"/>
       <c r="AE17" s="10"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
+    <row r="18" spans="1:31">
+      <c r="A18" s="51"/>
       <c r="B18" s="10"/>
       <c r="C18" s="32"/>
       <c r="D18" s="10"/>
@@ -4828,8 +4856,8 @@
       <c r="AD18" s="10"/>
       <c r="AE18" s="10"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
+    <row r="19" spans="1:31">
+      <c r="A19" s="51"/>
       <c r="B19" s="10"/>
       <c r="C19" s="32"/>
       <c r="D19" s="10"/>
@@ -4853,8 +4881,8 @@
       <c r="AD19" s="10"/>
       <c r="AE19" s="10"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="47"/>
+    <row r="20" spans="1:31">
+      <c r="A20" s="51"/>
       <c r="B20" s="10"/>
       <c r="C20" s="32"/>
       <c r="D20" s="10"/>
@@ -4865,7 +4893,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="33"/>
       <c r="K20" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="10"/>
@@ -4880,7 +4908,7 @@
       <c r="AD20" s="10"/>
       <c r="AE20" s="10"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31">
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="33"/>
@@ -4898,7 +4926,7 @@
       <c r="AD21" s="10"/>
       <c r="AE21" s="10"/>
     </row>
-    <row r="22" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" ht="15.95" customHeight="1">
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="17"/>
@@ -4916,7 +4944,7 @@
       <c r="AD22" s="10"/>
       <c r="AE22" s="10"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31">
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="17"/>
@@ -4936,7 +4964,7 @@
       <c r="AD23" s="10"/>
       <c r="AE23" s="10"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31">
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="17"/>
@@ -4956,7 +4984,7 @@
       <c r="AD24" s="10"/>
       <c r="AE24" s="10"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31">
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="17"/>
@@ -4967,7 +4995,7 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31">
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="17"/>
@@ -4975,70 +5003,70 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="121" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" ht="86.25">
       <c r="H27" s="10"/>
       <c r="J27" t="s">
-        <v>196</v>
-      </c>
-      <c r="K27" s="49" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="28" spans="1:31" ht="46" x14ac:dyDescent="0.2">
+      <c r="K27" s="47" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="29.25">
       <c r="J28" t="s">
         <v>151</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" ht="46" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="43.5">
       <c r="J29" t="s">
         <v>152</v>
       </c>
       <c r="K29" s="33" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="K30" s="9">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31">
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31">
       <c r="K32" s="9">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="48"/>
+    <row r="41" spans="1:13">
+      <c r="A41" s="46"/>
       <c r="B41" s="24"/>
       <c r="C41" s="32"/>
       <c r="D41" s="33"/>
@@ -5047,8 +5075,8 @@
       <c r="G41" s="32"/>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="48"/>
+    <row r="42" spans="1:13">
+      <c r="A42" s="46"/>
       <c r="B42" s="24"/>
       <c r="C42" s="32"/>
       <c r="D42" s="33"/>
@@ -5057,8 +5085,8 @@
       <c r="G42" s="32"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="48"/>
+    <row r="43" spans="1:13">
+      <c r="A43" s="46"/>
       <c r="B43" s="24"/>
       <c r="C43" s="32"/>
       <c r="D43" s="33"/>
@@ -5067,8 +5095,8 @@
       <c r="G43" s="32"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
+    <row r="44" spans="1:13">
+      <c r="A44" s="46"/>
       <c r="B44" s="24"/>
       <c r="C44" s="36"/>
       <c r="D44" s="33"/>
@@ -5077,7 +5105,7 @@
       <c r="G44" s="43"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
       <c r="D45" s="24"/>
@@ -5086,7 +5114,7 @@
       <c r="G45" s="24"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
       <c r="D46" s="24"/>
@@ -5118,47 +5146,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E602B0F9-DB71-6243-B91C-2D0F5CE0F4A2}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="24" t="s">
-        <v>165</v>
-      </c>
       <c r="G1" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1">
+      <c r="A2" s="50" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -5183,8 +5211,8 @@
       </c>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
+    <row r="3" spans="1:11">
+      <c r="A3" s="50"/>
       <c r="B3" s="23" t="s">
         <v>7</v>
       </c>
@@ -5207,13 +5235,13 @@
       </c>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
+    <row r="4" spans="1:11">
+      <c r="A4" s="50"/>
       <c r="B4" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="D4" s="23">
         <v>43.183140000000002</v>
@@ -5231,8 +5259,8 @@
       </c>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+    <row r="5" spans="1:11">
+      <c r="A5" s="50"/>
       <c r="B5" s="23" t="s">
         <v>148</v>
       </c>
@@ -5255,13 +5283,13 @@
       </c>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+    <row r="6" spans="1:11">
+      <c r="A6" s="50"/>
       <c r="B6" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D6" s="23">
         <v>44.954700000000003</v>
@@ -5279,8 +5307,8 @@
       </c>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+    <row r="7" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A7" s="50"/>
       <c r="B7" s="21" t="s">
         <v>149</v>
       </c>
@@ -5303,10 +5331,10 @@
       </c>
       <c r="H7" s="24"/>
     </row>
-    <row r="8" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
+    <row r="8" spans="1:11" ht="16.5" thickTop="1">
+      <c r="A8" s="50"/>
       <c r="B8" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="25">
         <v>0.89800000000000002</v>
@@ -5327,10 +5355,10 @@
       </c>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+    <row r="9" spans="1:11">
+      <c r="A9" s="50"/>
       <c r="B9" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" s="25">
         <v>0.91</v>
@@ -5351,13 +5379,13 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+    <row r="10" spans="1:11">
+      <c r="A10" s="50"/>
       <c r="B10" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="23">
         <v>46.423520000000003</v>
@@ -5375,13 +5403,13 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
+    <row r="11" spans="1:11">
+      <c r="A11" s="50"/>
       <c r="B11" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>184</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>185</v>
       </c>
       <c r="D11" s="23">
         <v>47.297080000000001</v>
@@ -5399,13 +5427,13 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
+    <row r="12" spans="1:11">
+      <c r="A12" s="50"/>
       <c r="B12" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>186</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>187</v>
       </c>
       <c r="D12" s="23">
         <v>57.785269999999997</v>
@@ -5423,15 +5451,15 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" s="50" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="D13" s="23">
         <v>55.85942</v>
@@ -5452,10 +5480,10 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+    <row r="14" spans="1:11">
+      <c r="A14" s="50"/>
       <c r="B14" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" s="24">
         <v>0.35099999999999998</v>
@@ -5479,8 +5507,8 @@
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+    <row r="15" spans="1:11">
+      <c r="A15" s="50"/>
       <c r="B15" s="23" t="s">
         <v>7</v>
       </c>
@@ -5506,8 +5534,8 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+    <row r="16" spans="1:11">
+      <c r="A16" s="50"/>
       <c r="B16" s="23" t="s">
         <v>149</v>
       </c>
@@ -5533,8 +5561,8 @@
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
+    <row r="17" spans="1:11">
+      <c r="A17" s="50"/>
       <c r="B17" s="23" t="s">
         <v>150</v>
       </c>
@@ -5560,10 +5588,10 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+    <row r="18" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A18" s="50"/>
       <c r="B18" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C18" s="22">
         <v>0.749</v>
@@ -5587,8 +5615,8 @@
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+    <row r="19" spans="1:11" ht="16.5" thickTop="1">
+      <c r="A19" s="50"/>
       <c r="B19" s="23" t="s">
         <v>148</v>
       </c>
@@ -5614,13 +5642,13 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
+    <row r="20" spans="1:11">
+      <c r="A20" s="50"/>
       <c r="B20" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D20" s="23">
         <v>61.300179999999997</v>
@@ -5641,13 +5669,13 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+    <row r="21" spans="1:11">
+      <c r="A21" s="50"/>
       <c r="B21" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D21" s="23">
         <v>61.951509999999999</v>
@@ -5668,13 +5696,13 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="46"/>
+    <row r="22" spans="1:11">
+      <c r="A22" s="50"/>
       <c r="B22" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D22" s="23">
         <v>62.24259</v>
@@ -5695,13 +5723,13 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="46"/>
+    <row r="23" spans="1:11">
+      <c r="A23" s="50"/>
       <c r="B23" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" s="23">
         <v>91.646410000000003</v>
@@ -5720,25 +5748,25 @@
       <c r="H23" s="10"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -5766,49 +5794,49 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="24" t="s">
-        <v>165</v>
-      </c>
       <c r="G1" s="25" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="D2" s="23">
         <v>55.85942</v>
@@ -5825,10 +5853,10 @@
         <v>0.3553945</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="45"/>
       <c r="B3" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3" s="24">
         <v>0.35099999999999998</v>
@@ -5848,7 +5876,7 @@
         <v>0.49708989999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="45"/>
       <c r="B4" s="23" t="s">
         <v>7</v>
@@ -5871,7 +5899,7 @@
         <v>0.59660057999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="45"/>
       <c r="B5" s="23" t="s">
         <v>149</v>
@@ -5894,7 +5922,7 @@
         <v>0.68659437999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="45"/>
       <c r="B6" s="23" t="s">
         <v>150</v>
@@ -5917,10 +5945,10 @@
         <v>0.77530591999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="16.5" thickBot="1">
       <c r="A7" s="45"/>
       <c r="B7" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="22">
         <v>0.749</v>
@@ -5940,7 +5968,7 @@
         <v>0.86274976000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="16.5" thickTop="1">
       <c r="A8" s="45"/>
       <c r="B8" s="23" t="s">
         <v>148</v>
@@ -5963,13 +5991,13 @@
         <v>0.94509052000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="45"/>
       <c r="B9" s="23" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D9" s="23">
         <v>61.300179999999997</v>
@@ -5986,13 +6014,13 @@
         <v>0.96849313000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="45"/>
       <c r="B10" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D10" s="23">
         <v>61.951509999999999</v>
@@ -6009,13 +6037,13 @@
         <v>0.98539093</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="45"/>
       <c r="B11" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" s="23">
         <v>62.24259</v>
@@ -6032,13 +6060,13 @@
         <v>1.0000000200000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="45"/>
       <c r="B12" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D12" s="23">
         <v>91.646410000000003</v>
@@ -6055,7 +6083,7 @@
         <v>1.0000000260209272</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
@@ -6063,18 +6091,18 @@
       <c r="F13" s="28"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:10">
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:10">
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -6082,7 +6110,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:10">
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -6090,7 +6118,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:10">
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -6098,7 +6126,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:10">
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -6106,7 +6134,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:10">
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -6114,7 +6142,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:10">
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -6122,7 +6150,7 @@
       <c r="I23" s="10"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:10">
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -6130,7 +6158,7 @@
       <c r="I24" s="10"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:10">
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -6138,31 +6166,31 @@
       <c r="I25" s="10"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:10">
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="17"/>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:10">
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:10">
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:10">
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:10">
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -6186,26 +6214,26 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D1" s="46" t="s">
+    <row r="1" spans="1:12">
+      <c r="D1" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
       <c r="L1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -6240,7 +6268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -6278,7 +6306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -6316,7 +6344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -6354,7 +6382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -6392,7 +6420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -6430,7 +6458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6468,7 +6496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -6506,7 +6534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -6544,7 +6572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -6582,7 +6610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -6620,7 +6648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -6658,7 +6686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -6696,7 +6724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -6734,7 +6762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -6772,7 +6800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -6810,7 +6838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -6848,7 +6876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -6886,7 +6914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -6924,15 +6952,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D22" s="46" t="s">
+    <row r="22" spans="1:12">
+      <c r="D22" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -6955,7 +6983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -6978,7 +7006,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -7001,7 +7029,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -7024,7 +7052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -7047,7 +7075,7 @@
         <v>0.218</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -7070,7 +7098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -7093,7 +7121,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -7116,7 +7144,7 @@
         <v>0.29499999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -7139,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -7162,7 +7190,7 @@
         <v>0.251</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -7185,7 +7213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -7208,7 +7236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -7231,7 +7259,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -7254,7 +7282,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -7277,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -7300,7 +7328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -7323,7 +7351,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -7346,7 +7374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -7383,29 +7411,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBFB128-21B5-574F-A98E-9FD81DFA13B6}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -7449,7 +7477,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -7493,7 +7521,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -7537,7 +7565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -7581,7 +7609,7 @@
         <v>9.0500000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -7625,7 +7653,7 @@
         <v>8.17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -7669,7 +7697,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -7713,7 +7741,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -7757,7 +7785,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -7801,7 +7829,7 @@
         <v>10.27</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -7845,7 +7873,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -7889,7 +7917,7 @@
         <v>14.74</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -7933,7 +7961,7 @@
         <v>16.55</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -7977,7 +8005,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -8021,7 +8049,7 @@
         <v>11.32</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -8065,7 +8093,7 @@
         <v>11.84</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -8109,7 +8137,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -8153,7 +8181,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -8197,7 +8225,7 @@
         <v>7.48</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>18</v>
       </c>

</xml_diff>